<commit_message>
230918, 230925, literacy modified
</commit_message>
<xml_diff>
--- a/R/data/literacy_230925.xlsx
+++ b/R/data/literacy_230925.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kwlee/My_Google_Drive/Works/Class/Statistics/R.WD/Class_data/class202302/R/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A443005-D65A-5443-AF02-EDE4D50F44D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D51EF724-5621-5B4D-9269-2BA0D2968E1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-33880" yWindow="580" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10277" uniqueCount="1002">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11573" uniqueCount="1100">
   <si>
     <t>타임스탬프</t>
   </si>
@@ -3029,6 +3029,300 @@
   </si>
   <si>
     <t>최태웅</t>
+  </si>
+  <si>
+    <t>smiledjwj@naver.com</t>
+  </si>
+  <si>
+    <t>김지우</t>
+  </si>
+  <si>
+    <t>jangho5636@gmail.com</t>
+  </si>
+  <si>
+    <t>이장호</t>
+  </si>
+  <si>
+    <t>chlwnsgur1202@gmail.com</t>
+  </si>
+  <si>
+    <t>최준혁</t>
+  </si>
+  <si>
+    <t>p.pla1226@gmail.com</t>
+  </si>
+  <si>
+    <t>박성곤</t>
+  </si>
+  <si>
+    <t>ksnkty123@naver.com</t>
+  </si>
+  <si>
+    <t>김태윤</t>
+  </si>
+  <si>
+    <t>wjddmsqjqtk@naver.com</t>
+  </si>
+  <si>
+    <t>신정은</t>
+  </si>
+  <si>
+    <t>lin031215@naver.com</t>
+  </si>
+  <si>
+    <t>jinwon4725@naver.vom</t>
+  </si>
+  <si>
+    <t>장진원</t>
+  </si>
+  <si>
+    <t>sjy01041864550@gmail.com</t>
+  </si>
+  <si>
+    <t>서진영</t>
+  </si>
+  <si>
+    <t>canty0917@gmail.com</t>
+  </si>
+  <si>
+    <t>조민주</t>
+  </si>
+  <si>
+    <t>enjoy9675@gmail.com</t>
+  </si>
+  <si>
+    <t>곽아영</t>
+  </si>
+  <si>
+    <t>rkgus8286@naver.com</t>
+  </si>
+  <si>
+    <t>이주영</t>
+  </si>
+  <si>
+    <t>amdo0421@naver.com</t>
+  </si>
+  <si>
+    <t>이은빈</t>
+  </si>
+  <si>
+    <t>rin5920@naver.com</t>
+  </si>
+  <si>
+    <t>djcjfakstp@gmail.com</t>
+  </si>
+  <si>
+    <t>융합인재학부</t>
+  </si>
+  <si>
+    <t>어철</t>
+  </si>
+  <si>
+    <t>cdm990512@gmail.com</t>
+  </si>
+  <si>
+    <t>천동민</t>
+  </si>
+  <si>
+    <t>jsk8070@naver.com</t>
+  </si>
+  <si>
+    <t>김세아</t>
+  </si>
+  <si>
+    <t>leehakyung1207@gmail.com</t>
+  </si>
+  <si>
+    <t>이하경</t>
+  </si>
+  <si>
+    <t>iceflower082@gmail.com</t>
+  </si>
+  <si>
+    <t>한지우</t>
+  </si>
+  <si>
+    <t>t26a1@naver.com</t>
+  </si>
+  <si>
+    <t>반도체</t>
+  </si>
+  <si>
+    <t>신동한</t>
+  </si>
+  <si>
+    <t>mingye990410@naver.com</t>
+  </si>
+  <si>
+    <t>콘텐츠IT학과</t>
+  </si>
+  <si>
+    <t>yoogyeonggg@naver.com</t>
+  </si>
+  <si>
+    <t>최유경</t>
+  </si>
+  <si>
+    <t>leetaeyang00@gmail.com</t>
+  </si>
+  <si>
+    <t>이태양</t>
+  </si>
+  <si>
+    <t>yjh110951@gmail.com</t>
+  </si>
+  <si>
+    <t>유정훈</t>
+  </si>
+  <si>
+    <t>gmyeongju515@gmail.com</t>
+  </si>
+  <si>
+    <t>김명주</t>
+  </si>
+  <si>
+    <t>jhyeong234@naver.com</t>
+  </si>
+  <si>
+    <t>김준형</t>
+  </si>
+  <si>
+    <t>minhan3729@gmail.com</t>
+  </si>
+  <si>
+    <t>이민한</t>
+  </si>
+  <si>
+    <t>gilhk031111@naver.com</t>
+  </si>
+  <si>
+    <t>길혜균</t>
+  </si>
+  <si>
+    <t>vlxjvos2514@naver.com</t>
+  </si>
+  <si>
+    <t>홍성은</t>
+  </si>
+  <si>
+    <t>djdodhrghr@naver.com</t>
+  </si>
+  <si>
+    <t>융합신소재공학전공</t>
+  </si>
+  <si>
+    <t>송서현</t>
+  </si>
+  <si>
+    <t>kgy5988@naver.com</t>
+  </si>
+  <si>
+    <t>김진범</t>
+  </si>
+  <si>
+    <t>luis0815@naver.com</t>
+  </si>
+  <si>
+    <t>양지민</t>
+  </si>
+  <si>
+    <t>sang010516@naver.com</t>
+  </si>
+  <si>
+    <t>최상은</t>
+  </si>
+  <si>
+    <t>rhy0787@naver.com</t>
+  </si>
+  <si>
+    <t>유희영</t>
+  </si>
+  <si>
+    <t>kdy3921633@naver.com</t>
+  </si>
+  <si>
+    <t>cozyandrelaxing2@gmail.com</t>
+  </si>
+  <si>
+    <t>이성민</t>
+  </si>
+  <si>
+    <t>mng437@naver.com</t>
+  </si>
+  <si>
+    <t>김민규</t>
+  </si>
+  <si>
+    <t>parksiwoo1214@naver.com</t>
+  </si>
+  <si>
+    <t>박시우</t>
+  </si>
+  <si>
+    <t>srankhanwoo@gmail.com</t>
+  </si>
+  <si>
+    <t>최찬우</t>
+  </si>
+  <si>
+    <t>spb012@naver.com</t>
+  </si>
+  <si>
+    <t>모수빈</t>
+  </si>
+  <si>
+    <t>kdh01270102@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 법학과</t>
+  </si>
+  <si>
+    <t>lhe0209@naver.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">경영학과 </t>
+  </si>
+  <si>
+    <t>이하은</t>
+  </si>
+  <si>
+    <t>jinhwanjeong8@gmail.com</t>
+  </si>
+  <si>
+    <t>정진환</t>
+  </si>
+  <si>
+    <t>2003lsa@naver.com</t>
+  </si>
+  <si>
+    <t>이수아</t>
+  </si>
+  <si>
+    <t>seongmo0731@naver.com</t>
+  </si>
+  <si>
+    <t>조성모</t>
+  </si>
+  <si>
+    <t>gys5785@naver.com</t>
+  </si>
+  <si>
+    <t>고형승</t>
+  </si>
+  <si>
+    <t>20233824@hallym.ac.kr</t>
+  </si>
+  <si>
+    <t>안지영</t>
+  </si>
+  <si>
+    <t>at79711@naver.com</t>
+  </si>
+  <si>
+    <t>데이터사이언스</t>
+  </si>
+  <si>
+    <t>박재영</t>
   </si>
 </sst>
 </file>
@@ -3311,11 +3605,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AD379"/>
+  <dimension ref="A1:AD427"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A343" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C382" sqref="C382"/>
+      <pane ySplit="1" topLeftCell="A403" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C433" sqref="C433"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -38191,6 +38485,4422 @@
         <v>91</v>
       </c>
     </row>
+    <row r="380" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A380" s="2">
+        <v>45200.370524432874</v>
+      </c>
+      <c r="B380" s="1" t="s">
+        <v>1002</v>
+      </c>
+      <c r="C380" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="D380" s="1">
+        <v>20231511</v>
+      </c>
+      <c r="E380" s="1" t="s">
+        <v>1003</v>
+      </c>
+      <c r="F380" s="1">
+        <v>3</v>
+      </c>
+      <c r="G380" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H380" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I380" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J380" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="K380" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="L380" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="M380" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="N380" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="O380" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="P380" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q380" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="R380" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="S380" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="T380" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="U380" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="V380" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="W380" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="X380" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y380" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z380" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA380" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AB380" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC380" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD380" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="381" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A381" s="2">
+        <v>45200.403748622688</v>
+      </c>
+      <c r="B381" s="1" t="s">
+        <v>1004</v>
+      </c>
+      <c r="C381" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="D381" s="1">
+        <v>20161723</v>
+      </c>
+      <c r="E381" s="1" t="s">
+        <v>1005</v>
+      </c>
+      <c r="F381" s="1">
+        <v>3</v>
+      </c>
+      <c r="G381" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H381" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I381" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J381" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="K381" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="L381" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="M381" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="N381" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="O381" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="P381" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q381" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="R381" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="S381" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="T381" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="U381" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="V381" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="W381" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="X381" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y381" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="Z381" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="AA381" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB381" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC381" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD381" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="382" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A382" s="2">
+        <v>45200.424993773151</v>
+      </c>
+      <c r="B382" s="1" t="s">
+        <v>1006</v>
+      </c>
+      <c r="C382" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="D382" s="1">
+        <v>20236783</v>
+      </c>
+      <c r="E382" s="1" t="s">
+        <v>1007</v>
+      </c>
+      <c r="F382" s="1">
+        <v>3</v>
+      </c>
+      <c r="G382" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="H382" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I382" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J382" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="K382" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="L382" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="M382" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="N382" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="O382" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="P382" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q382" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="R382" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="S382" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="T382" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="U382" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="V382" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="W382" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="X382" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y382" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="Z382" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA382" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AB382" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC382" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="AD382" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="383" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A383" s="2">
+        <v>45200.439072141206</v>
+      </c>
+      <c r="B383" s="1" t="s">
+        <v>1008</v>
+      </c>
+      <c r="C383" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D383" s="1">
+        <v>20236127</v>
+      </c>
+      <c r="E383" s="1" t="s">
+        <v>1009</v>
+      </c>
+      <c r="F383" s="1">
+        <v>3</v>
+      </c>
+      <c r="G383" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H383" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I383" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J383" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="K383" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="L383" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="M383" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="N383" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="O383" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="P383" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q383" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="R383" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="S383" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="T383" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="U383" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="V383" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="W383" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="X383" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y383" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z383" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA383" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AB383" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC383" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD383" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="384" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A384" s="2">
+        <v>45200.440122245374</v>
+      </c>
+      <c r="B384" s="1" t="s">
+        <v>1010</v>
+      </c>
+      <c r="C384" s="1" t="s">
+        <v>455</v>
+      </c>
+      <c r="D384" s="1">
+        <v>20232526</v>
+      </c>
+      <c r="E384" s="1" t="s">
+        <v>1011</v>
+      </c>
+      <c r="F384" s="1">
+        <v>3</v>
+      </c>
+      <c r="G384" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="H384" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="I384" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J384" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="K384" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="L384" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="M384" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="N384" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="O384" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="P384" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="Q384" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="R384" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="S384" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="T384" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="U384" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="V384" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="W384" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="X384" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y384" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="Z384" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA384" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="AB384" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC384" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="AD384" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="385" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A385" s="2">
+        <v>45200.452729907411</v>
+      </c>
+      <c r="B385" s="1" t="s">
+        <v>1012</v>
+      </c>
+      <c r="C385" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="D385" s="1">
+        <v>20221714</v>
+      </c>
+      <c r="E385" s="1" t="s">
+        <v>1013</v>
+      </c>
+      <c r="F385" s="1">
+        <v>3</v>
+      </c>
+      <c r="G385" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H385" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I385" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J385" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="K385" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="L385" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="M385" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="N385" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="O385" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="P385" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q385" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="R385" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="S385" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="T385" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="U385" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="V385" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="W385" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="X385" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y385" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z385" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA385" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AB385" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC385" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD385" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="386" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A386" s="2">
+        <v>45200.453657615741</v>
+      </c>
+      <c r="B386" s="1" t="s">
+        <v>1014</v>
+      </c>
+      <c r="C386" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="D386" s="1">
+        <v>20222570</v>
+      </c>
+      <c r="E386" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="F386" s="1">
+        <v>3</v>
+      </c>
+      <c r="G386" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H386" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I386" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J386" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="K386" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="L386" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="M386" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="N386" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="O386" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="P386" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q386" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="R386" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="S386" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="T386" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="U386" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="V386" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="W386" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="X386" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y386" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z386" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA386" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AB386" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC386" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD386" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="387" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A387" s="2">
+        <v>45200.471678043978</v>
+      </c>
+      <c r="B387" s="1" t="s">
+        <v>1015</v>
+      </c>
+      <c r="C387" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="D387" s="1">
+        <v>20232355</v>
+      </c>
+      <c r="E387" s="1" t="s">
+        <v>1016</v>
+      </c>
+      <c r="F387" s="1">
+        <v>3</v>
+      </c>
+      <c r="G387" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="H387" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="I387" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J387" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="K387" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="L387" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="M387" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="N387" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="O387" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="P387" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q387" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="R387" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="S387" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="T387" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="U387" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="V387" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="W387" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="X387" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y387" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z387" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA387" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AB387" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC387" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD387" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="388" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A388" s="2">
+        <v>45200.482950659723</v>
+      </c>
+      <c r="B388" s="1" t="s">
+        <v>1017</v>
+      </c>
+      <c r="C388" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="D388" s="1">
+        <v>20236620</v>
+      </c>
+      <c r="E388" s="1" t="s">
+        <v>1018</v>
+      </c>
+      <c r="F388" s="1">
+        <v>3</v>
+      </c>
+      <c r="G388" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="H388" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="I388" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="J388" s="1" t="s">
+        <v>435</v>
+      </c>
+      <c r="K388" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="L388" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="M388" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="N388" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="O388" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="P388" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="Q388" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="R388" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="S388" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="T388" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="U388" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="V388" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="W388" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="X388" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="Y388" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="Z388" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="AA388" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AB388" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="AC388" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="AD388" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="389" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A389" s="2">
+        <v>45200.520382569448</v>
+      </c>
+      <c r="B389" s="1" t="s">
+        <v>1019</v>
+      </c>
+      <c r="C389" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="D389" s="1">
+        <v>20232363</v>
+      </c>
+      <c r="E389" s="1" t="s">
+        <v>1020</v>
+      </c>
+      <c r="F389" s="1">
+        <v>3</v>
+      </c>
+      <c r="G389" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H389" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I389" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J389" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="K389" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="L389" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="M389" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="N389" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="O389" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="P389" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q389" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="R389" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="S389" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="T389" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="U389" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="V389" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="W389" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="X389" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y389" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z389" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA389" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AB389" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC389" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD389" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="390" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A390" s="2">
+        <v>45200.523549872683</v>
+      </c>
+      <c r="B390" s="1" t="s">
+        <v>1021</v>
+      </c>
+      <c r="C390" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="D390" s="1">
+        <v>20213801</v>
+      </c>
+      <c r="E390" s="1" t="s">
+        <v>1022</v>
+      </c>
+      <c r="F390" s="1">
+        <v>3</v>
+      </c>
+      <c r="G390" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H390" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I390" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J390" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="K390" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="L390" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="M390" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="N390" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="O390" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="P390" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q390" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="R390" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="S390" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="T390" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="U390" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="V390" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="W390" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="X390" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y390" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z390" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA390" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="AB390" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC390" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD390" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="391" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A391" s="2">
+        <v>45200.537087546298</v>
+      </c>
+      <c r="B391" s="1" t="s">
+        <v>1023</v>
+      </c>
+      <c r="C391" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D391" s="1">
+        <v>20233729</v>
+      </c>
+      <c r="E391" s="1" t="s">
+        <v>1024</v>
+      </c>
+      <c r="F391" s="1">
+        <v>3</v>
+      </c>
+      <c r="G391" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H391" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I391" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J391" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="K391" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="L391" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="M391" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="N391" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="O391" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="P391" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q391" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="R391" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="S391" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="T391" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="U391" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="V391" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="W391" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="X391" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y391" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z391" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA391" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB391" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC391" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD391" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="392" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A392" s="2">
+        <v>45200.554801979168</v>
+      </c>
+      <c r="B392" s="1" t="s">
+        <v>1025</v>
+      </c>
+      <c r="C392" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D392" s="1">
+        <v>20236278</v>
+      </c>
+      <c r="E392" s="1" t="s">
+        <v>1026</v>
+      </c>
+      <c r="F392" s="1">
+        <v>3</v>
+      </c>
+      <c r="G392" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H392" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I392" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J392" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="K392" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="L392" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="M392" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="N392" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="O392" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="P392" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q392" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="R392" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="S392" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="T392" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="U392" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="V392" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="W392" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="X392" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y392" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z392" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA392" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB392" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC392" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD392" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="393" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A393" s="2">
+        <v>45200.557146689811</v>
+      </c>
+      <c r="B393" s="1" t="s">
+        <v>1027</v>
+      </c>
+      <c r="C393" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="D393" s="1">
+        <v>20233425</v>
+      </c>
+      <c r="E393" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="F393" s="1">
+        <v>3</v>
+      </c>
+      <c r="G393" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H393" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I393" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J393" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="K393" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="L393" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="M393" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="N393" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="O393" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="P393" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q393" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="R393" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="S393" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="T393" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="U393" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="V393" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="W393" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="X393" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y393" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z393" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA393" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AB393" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC393" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD393" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="394" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A394" s="2">
+        <v>45200.562361435186</v>
+      </c>
+      <c r="B394" s="1" t="s">
+        <v>1028</v>
+      </c>
+      <c r="C394" s="1" t="s">
+        <v>1029</v>
+      </c>
+      <c r="D394" s="1">
+        <v>20196515</v>
+      </c>
+      <c r="E394" s="1" t="s">
+        <v>1030</v>
+      </c>
+      <c r="F394" s="1">
+        <v>3</v>
+      </c>
+      <c r="G394" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H394" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="I394" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J394" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="K394" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="L394" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="M394" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="N394" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="O394" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="P394" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="Q394" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="R394" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="S394" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="T394" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="U394" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="V394" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="W394" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="X394" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y394" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z394" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="AA394" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AB394" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="AC394" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="AD394" s="1" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="395" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A395" s="2">
+        <v>45200.568709224535</v>
+      </c>
+      <c r="B395" s="1" t="s">
+        <v>1031</v>
+      </c>
+      <c r="C395" s="1" t="s">
+        <v>659</v>
+      </c>
+      <c r="D395" s="1">
+        <v>20185300</v>
+      </c>
+      <c r="E395" s="1" t="s">
+        <v>1032</v>
+      </c>
+      <c r="F395" s="1">
+        <v>3</v>
+      </c>
+      <c r="G395" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H395" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I395" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J395" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="K395" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="L395" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="M395" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="N395" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="O395" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="P395" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q395" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="R395" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="S395" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="T395" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="U395" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="V395" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="W395" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="X395" s="1" t="s">
+        <v>436</v>
+      </c>
+      <c r="Y395" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="Z395" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="AA395" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB395" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="AC395" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD395" s="1" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="396" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A396" s="2">
+        <v>45200.569775706019</v>
+      </c>
+      <c r="B396" s="1" t="s">
+        <v>1033</v>
+      </c>
+      <c r="C396" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D396" s="1">
+        <v>20207064</v>
+      </c>
+      <c r="E396" s="1" t="s">
+        <v>1034</v>
+      </c>
+      <c r="F396" s="1">
+        <v>3</v>
+      </c>
+      <c r="G396" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H396" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I396" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J396" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="K396" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="L396" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="M396" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="N396" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="O396" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="P396" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q396" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="R396" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="S396" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="T396" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="U396" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="V396" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="W396" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="X396" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y396" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z396" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA396" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AB396" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC396" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD396" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="397" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A397" s="2">
+        <v>45200.570516898151</v>
+      </c>
+      <c r="B397" s="1" t="s">
+        <v>1035</v>
+      </c>
+      <c r="C397" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="D397" s="1">
+        <v>20235245</v>
+      </c>
+      <c r="E397" s="1" t="s">
+        <v>1036</v>
+      </c>
+      <c r="F397" s="1">
+        <v>3</v>
+      </c>
+      <c r="G397" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H397" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I397" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J397" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="K397" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="L397" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="M397" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="N397" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="O397" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="P397" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q397" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="R397" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="S397" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="T397" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="U397" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="V397" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="W397" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="X397" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y397" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z397" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA397" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AB397" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC397" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="AD397" s="1" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="398" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A398" s="2">
+        <v>45200.571266458333</v>
+      </c>
+      <c r="B398" s="1" t="s">
+        <v>1037</v>
+      </c>
+      <c r="C398" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="D398" s="1">
+        <v>20226647</v>
+      </c>
+      <c r="E398" s="1" t="s">
+        <v>1038</v>
+      </c>
+      <c r="F398" s="1">
+        <v>2</v>
+      </c>
+      <c r="G398" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H398" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I398" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J398" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="K398" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="L398" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="M398" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="N398" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="O398" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="P398" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q398" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="R398" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="S398" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="T398" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="U398" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="V398" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="W398" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="X398" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y398" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z398" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA398" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AB398" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC398" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD398" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="399" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A399" s="2">
+        <v>45200.586571817126</v>
+      </c>
+      <c r="B399" s="1" t="s">
+        <v>1039</v>
+      </c>
+      <c r="C399" s="1" t="s">
+        <v>1040</v>
+      </c>
+      <c r="D399" s="1">
+        <v>20193331</v>
+      </c>
+      <c r="E399" s="1" t="s">
+        <v>1041</v>
+      </c>
+      <c r="F399" s="1">
+        <v>2</v>
+      </c>
+      <c r="G399" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H399" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I399" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J399" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="K399" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="L399" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="M399" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="N399" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="O399" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="P399" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q399" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="R399" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="S399" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="T399" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="U399" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="V399" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="W399" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="X399" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y399" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z399" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA399" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AB399" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC399" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD399" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="400" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A400" s="2">
+        <v>45200.598379722222</v>
+      </c>
+      <c r="B400" s="1" t="s">
+        <v>1042</v>
+      </c>
+      <c r="C400" s="1" t="s">
+        <v>1043</v>
+      </c>
+      <c r="D400" s="1">
+        <v>20183639</v>
+      </c>
+      <c r="E400" s="1" t="s">
+        <v>700</v>
+      </c>
+      <c r="F400" s="1">
+        <v>3</v>
+      </c>
+      <c r="G400" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H400" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I400" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J400" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="K400" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="L400" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="M400" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="N400" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="O400" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="P400" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q400" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="R400" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="S400" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="T400" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="U400" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="V400" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="W400" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="X400" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y400" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z400" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA400" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AB400" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC400" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD400" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="401" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A401" s="2">
+        <v>45200.605743287037</v>
+      </c>
+      <c r="B401" s="1" t="s">
+        <v>1044</v>
+      </c>
+      <c r="C401" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="D401" s="1">
+        <v>20231238</v>
+      </c>
+      <c r="E401" s="1" t="s">
+        <v>1045</v>
+      </c>
+      <c r="F401" s="1">
+        <v>3</v>
+      </c>
+      <c r="G401" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="H401" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="I401" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="J401" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="K401" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="L401" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="M401" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="N401" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="O401" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="P401" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="Q401" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="R401" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="S401" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="T401" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="U401" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="V401" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="W401" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="X401" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="Y401" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="Z401" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="AA401" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AB401" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="AC401" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD401" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="402" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A402" s="2">
+        <v>45200.615215300924</v>
+      </c>
+      <c r="B402" s="1" t="s">
+        <v>1046</v>
+      </c>
+      <c r="C402" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="D402" s="1">
+        <v>20236764</v>
+      </c>
+      <c r="E402" s="1" t="s">
+        <v>1047</v>
+      </c>
+      <c r="F402" s="1">
+        <v>3</v>
+      </c>
+      <c r="G402" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H402" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I402" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J402" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="K402" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="L402" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="M402" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="N402" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="O402" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="P402" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q402" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="R402" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="S402" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="T402" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="U402" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="V402" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="W402" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="X402" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="Y402" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="Z402" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA402" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="AB402" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="AC402" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD402" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="403" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A403" s="2">
+        <v>45200.615888333334</v>
+      </c>
+      <c r="B403" s="1" t="s">
+        <v>1048</v>
+      </c>
+      <c r="C403" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D403" s="1">
+        <v>20232995</v>
+      </c>
+      <c r="E403" s="1" t="s">
+        <v>1049</v>
+      </c>
+      <c r="F403" s="1">
+        <v>3</v>
+      </c>
+      <c r="G403" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H403" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I403" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J403" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="K403" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="L403" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="M403" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="N403" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="O403" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="P403" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q403" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="R403" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="S403" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="T403" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="U403" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="V403" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="W403" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="X403" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y403" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z403" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA403" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AB403" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC403" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD403" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="404" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A404" s="2">
+        <v>45200.636823553243</v>
+      </c>
+      <c r="B404" s="1" t="s">
+        <v>1050</v>
+      </c>
+      <c r="C404" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="D404" s="1">
+        <v>20213606</v>
+      </c>
+      <c r="E404" s="1" t="s">
+        <v>1051</v>
+      </c>
+      <c r="F404" s="1">
+        <v>3</v>
+      </c>
+      <c r="G404" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H404" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I404" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J404" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="K404" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="L404" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="M404" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="N404" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="O404" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="P404" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q404" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="R404" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="S404" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="T404" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="U404" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="V404" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="W404" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="X404" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y404" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z404" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA404" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AB404" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC404" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD404" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="405" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A405" s="2">
+        <v>45200.645205451394</v>
+      </c>
+      <c r="B405" s="1" t="s">
+        <v>1052</v>
+      </c>
+      <c r="C405" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="D405" s="1">
+        <v>20232935</v>
+      </c>
+      <c r="E405" s="1" t="s">
+        <v>1053</v>
+      </c>
+      <c r="F405" s="1">
+        <v>3</v>
+      </c>
+      <c r="G405" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H405" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="I405" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J405" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="K405" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="L405" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="M405" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="N405" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="O405" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="P405" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q405" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="R405" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="S405" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="T405" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="U405" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="V405" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="W405" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="X405" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y405" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="Z405" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA405" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB405" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC405" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="AD405" s="1" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="406" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A406" s="2">
+        <v>45200.645880069445</v>
+      </c>
+      <c r="B406" s="1" t="s">
+        <v>1054</v>
+      </c>
+      <c r="C406" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="D406" s="1">
+        <v>20182556</v>
+      </c>
+      <c r="E406" s="1" t="s">
+        <v>1055</v>
+      </c>
+      <c r="F406" s="1">
+        <v>3</v>
+      </c>
+      <c r="G406" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H406" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I406" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J406" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="K406" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="L406" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="M406" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="N406" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="O406" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="P406" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q406" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="R406" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="S406" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="T406" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="U406" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="V406" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="W406" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="X406" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y406" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="Z406" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA406" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB406" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC406" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD406" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="407" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A407" s="2">
+        <v>45200.668389212966</v>
+      </c>
+      <c r="B407" s="1" t="s">
+        <v>1056</v>
+      </c>
+      <c r="C407" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="D407" s="1">
+        <v>20233204</v>
+      </c>
+      <c r="E407" s="1" t="s">
+        <v>1057</v>
+      </c>
+      <c r="F407" s="1">
+        <v>3</v>
+      </c>
+      <c r="G407" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H407" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="I407" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J407" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="K407" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="L407" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="M407" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="N407" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="O407" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="P407" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q407" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="R407" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="S407" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="T407" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="U407" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="V407" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="W407" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="X407" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y407" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="Z407" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="AA407" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AB407" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC407" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="AD407" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="408" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A408" s="2">
+        <v>45200.6738615625</v>
+      </c>
+      <c r="B408" s="1" t="s">
+        <v>1058</v>
+      </c>
+      <c r="C408" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D408" s="1">
+        <v>20203739</v>
+      </c>
+      <c r="E408" s="1" t="s">
+        <v>1059</v>
+      </c>
+      <c r="F408" s="1">
+        <v>3</v>
+      </c>
+      <c r="G408" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="H408" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I408" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J408" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="K408" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="L408" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="M408" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="N408" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="O408" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="P408" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q408" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="R408" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="S408" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="T408" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="U408" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="V408" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="W408" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="X408" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y408" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z408" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="AA408" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AB408" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC408" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="AD408" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="409" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A409" s="2">
+        <v>45200.676431990738</v>
+      </c>
+      <c r="B409" s="1" t="s">
+        <v>1060</v>
+      </c>
+      <c r="C409" s="1" t="s">
+        <v>1061</v>
+      </c>
+      <c r="D409" s="1">
+        <v>20216618</v>
+      </c>
+      <c r="E409" s="1" t="s">
+        <v>1062</v>
+      </c>
+      <c r="F409" s="1">
+        <v>3</v>
+      </c>
+      <c r="G409" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H409" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I409" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J409" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="K409" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="L409" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="M409" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="N409" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="O409" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="P409" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q409" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="R409" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="S409" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="T409" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="U409" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="V409" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="W409" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="X409" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y409" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z409" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA409" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB409" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC409" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD409" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="410" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A410" s="2">
+        <v>45200.693341597223</v>
+      </c>
+      <c r="B410" s="1" t="s">
+        <v>1063</v>
+      </c>
+      <c r="C410" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="D410" s="1">
+        <v>20203214</v>
+      </c>
+      <c r="E410" s="1" t="s">
+        <v>1064</v>
+      </c>
+      <c r="F410" s="1">
+        <v>3</v>
+      </c>
+      <c r="G410" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H410" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I410" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J410" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="K410" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="L410" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="M410" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="N410" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="O410" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="P410" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q410" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="R410" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="S410" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="T410" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="U410" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="V410" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="W410" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="X410" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y410" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="Z410" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA410" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AB410" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC410" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD410" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="411" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A411" s="2">
+        <v>45200.694757256948</v>
+      </c>
+      <c r="B411" s="1" t="s">
+        <v>1065</v>
+      </c>
+      <c r="C411" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="D411" s="1">
+        <v>20232336</v>
+      </c>
+      <c r="E411" s="1" t="s">
+        <v>1066</v>
+      </c>
+      <c r="F411" s="1">
+        <v>3</v>
+      </c>
+      <c r="G411" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H411" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I411" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J411" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="K411" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="L411" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="M411" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="N411" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="O411" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="P411" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q411" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="R411" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="S411" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="T411" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="U411" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="V411" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="W411" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="X411" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y411" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z411" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="AA411" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AB411" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC411" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD411" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="412" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A412" s="2">
+        <v>45200.698147627314</v>
+      </c>
+      <c r="B412" s="1" t="s">
+        <v>1067</v>
+      </c>
+      <c r="C412" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D412" s="1">
+        <v>20202851</v>
+      </c>
+      <c r="E412" s="1" t="s">
+        <v>1068</v>
+      </c>
+      <c r="F412" s="1">
+        <v>3</v>
+      </c>
+      <c r="G412" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H412" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I412" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J412" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="K412" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="L412" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="M412" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="N412" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="O412" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="P412" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q412" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="R412" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="S412" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="T412" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="U412" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="V412" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="W412" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="X412" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y412" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z412" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA412" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AB412" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="AC412" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD412" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="413" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A413" s="2">
+        <v>45200.705038530097</v>
+      </c>
+      <c r="B413" s="1" t="s">
+        <v>1069</v>
+      </c>
+      <c r="C413" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D413" s="1">
+        <v>20213827</v>
+      </c>
+      <c r="E413" s="1" t="s">
+        <v>1070</v>
+      </c>
+      <c r="F413" s="1">
+        <v>3</v>
+      </c>
+      <c r="G413" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H413" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I413" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J413" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="K413" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="L413" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="M413" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="N413" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="O413" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="P413" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q413" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="R413" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="S413" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="T413" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="U413" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="V413" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="W413" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="X413" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y413" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z413" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA413" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AB413" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC413" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD413" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="414" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A414" s="2">
+        <v>45200.713617766203</v>
+      </c>
+      <c r="B414" s="1" t="s">
+        <v>1071</v>
+      </c>
+      <c r="C414" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D414" s="1">
+        <v>20232604</v>
+      </c>
+      <c r="E414" s="1" t="s">
+        <v>660</v>
+      </c>
+      <c r="F414" s="1">
+        <v>3</v>
+      </c>
+      <c r="G414" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H414" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I414" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J414" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="K414" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="L414" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="M414" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="N414" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="O414" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="P414" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q414" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="R414" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="S414" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="T414" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="U414" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="V414" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="W414" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="X414" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y414" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="Z414" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA414" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="AB414" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC414" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="AD414" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="415" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A415" s="2">
+        <v>45200.716969618057</v>
+      </c>
+      <c r="B415" s="1" t="s">
+        <v>1072</v>
+      </c>
+      <c r="C415" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D415" s="1">
+        <v>20223725</v>
+      </c>
+      <c r="E415" s="1" t="s">
+        <v>1073</v>
+      </c>
+      <c r="F415" s="1">
+        <v>3</v>
+      </c>
+      <c r="G415" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H415" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I415" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J415" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="K415" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="L415" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="M415" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="N415" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="O415" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="P415" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q415" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="R415" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="S415" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="T415" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="U415" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="V415" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="W415" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="X415" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y415" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z415" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA415" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AB415" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC415" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD415" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="416" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A416" s="2">
+        <v>45200.719717858796</v>
+      </c>
+      <c r="B416" s="1" t="s">
+        <v>1074</v>
+      </c>
+      <c r="C416" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="D416" s="1">
+        <v>20232105</v>
+      </c>
+      <c r="E416" s="1" t="s">
+        <v>1075</v>
+      </c>
+      <c r="F416" s="1">
+        <v>3</v>
+      </c>
+      <c r="G416" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="H416" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I416" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J416" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="K416" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="L416" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="M416" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="N416" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="O416" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="P416" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q416" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="R416" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="S416" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="T416" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="U416" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="V416" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="W416" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="X416" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y416" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="Z416" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA416" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB416" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC416" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD416" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="417" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A417" s="2">
+        <v>45200.722458611112</v>
+      </c>
+      <c r="B417" s="1" t="s">
+        <v>1076</v>
+      </c>
+      <c r="C417" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="D417" s="1">
+        <v>20193219</v>
+      </c>
+      <c r="E417" s="1" t="s">
+        <v>1077</v>
+      </c>
+      <c r="F417" s="1">
+        <v>3</v>
+      </c>
+      <c r="G417" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H417" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I417" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J417" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="K417" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="L417" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="M417" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="N417" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="O417" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="P417" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q417" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="R417" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="S417" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="T417" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="U417" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="V417" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="W417" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="X417" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y417" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z417" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA417" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AB417" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC417" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD417" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="418" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A418" s="2">
+        <v>45200.740926863422</v>
+      </c>
+      <c r="B418" s="1" t="s">
+        <v>1078</v>
+      </c>
+      <c r="C418" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D418" s="1">
+        <v>20226175</v>
+      </c>
+      <c r="E418" s="1" t="s">
+        <v>1079</v>
+      </c>
+      <c r="F418" s="1">
+        <v>3</v>
+      </c>
+      <c r="G418" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H418" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I418" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J418" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="K418" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="L418" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="M418" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="N418" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="O418" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="P418" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q418" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="R418" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="S418" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="T418" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="U418" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="V418" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="W418" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="X418" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y418" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z418" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA418" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AB418" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC418" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD418" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="419" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A419" s="2">
+        <v>45200.742400370371</v>
+      </c>
+      <c r="B419" s="1" t="s">
+        <v>1080</v>
+      </c>
+      <c r="C419" s="1" t="s">
+        <v>455</v>
+      </c>
+      <c r="D419" s="1">
+        <v>20232530</v>
+      </c>
+      <c r="E419" s="1" t="s">
+        <v>1081</v>
+      </c>
+      <c r="F419" s="1">
+        <v>3</v>
+      </c>
+      <c r="G419" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H419" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I419" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J419" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="K419" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="L419" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="M419" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="N419" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="O419" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="P419" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q419" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="R419" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="S419" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="T419" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="U419" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="V419" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="W419" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="X419" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y419" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z419" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="AA419" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AB419" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC419" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD419" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="420" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A420" s="2">
+        <v>45200.743360995373</v>
+      </c>
+      <c r="B420" s="1" t="s">
+        <v>1082</v>
+      </c>
+      <c r="C420" s="1" t="s">
+        <v>1083</v>
+      </c>
+      <c r="D420" s="1">
+        <v>20212707</v>
+      </c>
+      <c r="E420" s="1" t="s">
+        <v>953</v>
+      </c>
+      <c r="F420" s="1">
+        <v>3</v>
+      </c>
+      <c r="G420" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="H420" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="I420" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="J420" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="K420" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="L420" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="M420" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="N420" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="O420" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="P420" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="Q420" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="R420" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="S420" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="T420" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="U420" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="V420" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="W420" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="X420" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="Y420" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="Z420" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA420" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB420" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="AC420" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="AD420" s="1" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="421" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A421" s="2">
+        <v>45200.74615204861</v>
+      </c>
+      <c r="B421" s="1" t="s">
+        <v>1084</v>
+      </c>
+      <c r="C421" s="1" t="s">
+        <v>1085</v>
+      </c>
+      <c r="D421" s="1">
+        <v>20213024</v>
+      </c>
+      <c r="E421" s="1" t="s">
+        <v>1086</v>
+      </c>
+      <c r="F421" s="1">
+        <v>3</v>
+      </c>
+      <c r="G421" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H421" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I421" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J421" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="K421" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="L421" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="M421" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="N421" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="O421" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="P421" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q421" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="R421" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="S421" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="T421" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="U421" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="V421" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="W421" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="X421" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y421" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z421" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA421" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB421" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC421" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD421" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="422" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A422" s="2">
+        <v>45200.751961863425</v>
+      </c>
+      <c r="B422" s="1" t="s">
+        <v>1087</v>
+      </c>
+      <c r="C422" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="D422" s="1">
+        <v>20236776</v>
+      </c>
+      <c r="E422" s="1" t="s">
+        <v>1088</v>
+      </c>
+      <c r="F422" s="1">
+        <v>3</v>
+      </c>
+      <c r="G422" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H422" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="I422" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J422" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="K422" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="L422" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="M422" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="N422" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="O422" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="P422" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q422" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="R422" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="S422" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="T422" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="U422" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="V422" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="W422" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="X422" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y422" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z422" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA422" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AB422" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC422" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD422" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="423" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A423" s="2">
+        <v>45200.753916828704</v>
+      </c>
+      <c r="B423" s="1" t="s">
+        <v>1089</v>
+      </c>
+      <c r="C423" s="1" t="s">
+        <v>1085</v>
+      </c>
+      <c r="D423" s="1">
+        <v>20223000</v>
+      </c>
+      <c r="E423" s="1" t="s">
+        <v>1090</v>
+      </c>
+      <c r="F423" s="1">
+        <v>3</v>
+      </c>
+      <c r="G423" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H423" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I423" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J423" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="K423" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="L423" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="M423" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="N423" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="O423" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="P423" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q423" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="R423" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="S423" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="T423" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="U423" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="V423" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="W423" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="X423" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y423" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z423" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA423" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AB423" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC423" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD423" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="424" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A424" s="2">
+        <v>45200.758232210646</v>
+      </c>
+      <c r="B424" s="1" t="s">
+        <v>1091</v>
+      </c>
+      <c r="C424" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D424" s="1">
+        <v>20192988</v>
+      </c>
+      <c r="E424" s="1" t="s">
+        <v>1092</v>
+      </c>
+      <c r="F424" s="1">
+        <v>3</v>
+      </c>
+      <c r="G424" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H424" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I424" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J424" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="K424" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="L424" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="M424" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="N424" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="O424" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="P424" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q424" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="R424" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="S424" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="T424" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="U424" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="V424" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="W424" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="X424" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y424" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z424" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA424" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AB424" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC424" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD424" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="425" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A425" s="2">
+        <v>45200.75969600695</v>
+      </c>
+      <c r="B425" s="1" t="s">
+        <v>1093</v>
+      </c>
+      <c r="C425" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="D425" s="1">
+        <v>20232402</v>
+      </c>
+      <c r="E425" s="1" t="s">
+        <v>1094</v>
+      </c>
+      <c r="F425" s="1">
+        <v>3</v>
+      </c>
+      <c r="G425" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H425" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I425" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J425" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="K425" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="L425" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="M425" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="N425" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="O425" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="P425" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q425" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="R425" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="S425" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="T425" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="U425" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="V425" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="W425" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="X425" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y425" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z425" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA425" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AB425" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC425" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="AD425" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="426" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A426" s="2">
+        <v>45200.76239131944</v>
+      </c>
+      <c r="B426" s="1" t="s">
+        <v>1095</v>
+      </c>
+      <c r="C426" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D426" s="1">
+        <v>20233824</v>
+      </c>
+      <c r="E426" s="1" t="s">
+        <v>1096</v>
+      </c>
+      <c r="F426" s="1">
+        <v>3</v>
+      </c>
+      <c r="G426" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="H426" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I426" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J426" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="K426" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="L426" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="M426" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="N426" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="O426" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="P426" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q426" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="R426" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="S426" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="T426" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="U426" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="V426" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="W426" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="X426" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y426" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z426" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="AA426" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AB426" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC426" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD426" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="427" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A427" s="2">
+        <v>45200.772507939815</v>
+      </c>
+      <c r="B427" s="1" t="s">
+        <v>1097</v>
+      </c>
+      <c r="C427" s="1" t="s">
+        <v>1098</v>
+      </c>
+      <c r="D427" s="1">
+        <v>20233220</v>
+      </c>
+      <c r="E427" s="1" t="s">
+        <v>1099</v>
+      </c>
+      <c r="F427" s="1">
+        <v>1</v>
+      </c>
+      <c r="G427" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H427" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I427" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J427" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="K427" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="L427" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="M427" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="N427" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="O427" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="P427" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q427" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="R427" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="S427" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="T427" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="U427" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="V427" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="W427" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="X427" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y427" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z427" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA427" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AB427" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC427" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD427" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>